<commit_message>
-manage data input output folder
</commit_message>
<xml_diff>
--- a/tugboat_schedule_v3.xlsx
+++ b/tugboat_schedule_v3.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Timeline" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Summary!$A$1:$T$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Summary!$A$1:$S$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Timeline!$A$3:$E$3</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -29229,7 +29229,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T1"/>
+  <autoFilter ref="A1:S1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>